<commit_message>
modif etudiant et classe
</commit_message>
<xml_diff>
--- a/memo.xlsx
+++ b/memo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Doc_jor\CGIInstitut\GIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Doc_jor\CGIInstitut\GIT\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="133">
   <si>
     <t>Mot clé/script</t>
   </si>
@@ -487,6 +487,12 @@
   </si>
   <si>
     <t>A voir un peu plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git diff --cached </t>
+  </si>
+  <si>
+    <t>Permet d'avoir la différence des modifs ajoutés sur les fichiers indexés</t>
   </si>
 </sst>
 </file>
@@ -893,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B68" activeCellId="1" sqref="B73 B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1499,8 +1505,12 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
+      <c r="A67" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="C67" s="2"/>
     </row>
   </sheetData>

</xml_diff>